<commit_message>
Work on grade tables: composite calculation
</commit_message>
<xml_diff>
--- a/TESTDATA/testing/Noten/NOTEN_1/Noten_12G.R_1.xlsx
+++ b/TESTDATA/testing/Noten/NOTEN_1/Noten_12G.R_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t xml:space="preserve">Notentabelle, erstellt 2022-01-04 16:52</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rudolf Rändier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.74"/>
@@ -1066,14 +1072,12 @@
         <v>15</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>61</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="R14" s="19"/>
       <c r="S14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1126,13 +1130,17 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="N4:S4"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S11:AD14 E15:AD52" type="list">
       <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*,/"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11:R14" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11:R13 E14:P14 R14" type="list">
       <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*,/"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q14" type="list">
+      <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*,/,X"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>